<commit_message>
packing perlengkapan PDH dan BN
</commit_message>
<xml_diff>
--- a/4. PDH DP 3N30 (MERAH) 3T25(COKLAT MUDA) 4N31(PUTIH) 5N38(HIJAU TUA) 5T38(PINKMUDA)/SUDAH UKUR DP4N31 TMT 12022021.xlsx
+++ b/4. PDH DP 3N30 (MERAH) 3T25(COKLAT MUDA) 4N31(PUTIH) 5N38(HIJAU TUA) 5T38(PINKMUDA)/SUDAH UKUR DP4N31 TMT 12022021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="123820"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\4. PDH DP 3N30 (MERAH) 3T25(COKLAT MUDA) 4N31(PUTIH) 5N38(HIJAU TUA) 5T38(PINKMUDA)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73BE968-FE1A-47A9-824B-50FE4D06D6B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8203B2-ACCC-4426-A389-51F84C12708C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="43">
   <si>
     <t>ABU NAWAS</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>MARLION</t>
+  </si>
+  <si>
+    <t>EDI SATRIYO</t>
   </si>
 </sst>
 </file>
@@ -215,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -246,6 +249,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -582,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1210,30 +1216,31 @@
     </row>
     <row r="30" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E30" s="6">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F30" s="6">
-        <v>56</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="G30" s="11"/>
     </row>
     <row r="31" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>1</v>
@@ -1242,18 +1249,18 @@
         <v>2</v>
       </c>
       <c r="E31" s="6">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F31" s="6">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>1</v>
@@ -1270,26 +1277,30 @@
     </row>
     <row r="33" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
-        <v>33</v>
-      </c>
-      <c r="B33" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="6">
         <v>41</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
+      <c r="F33" s="6">
+        <v>55</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>1</v>
@@ -1297,28 +1308,52 @@
       <c r="D34" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="8">
-        <v>43</v>
-      </c>
-      <c r="F34" s="8">
-        <v>60</v>
+      <c r="E34" s="9">
+        <v>42</v>
+      </c>
+      <c r="F34" s="9">
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="8">
+        <v>43</v>
+      </c>
+      <c r="F35" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
         <v>35</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B36" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
+      <c r="C36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="9">
+        <v>44</v>
+      </c>
+      <c r="F36" s="9">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.45" bottom="0.33" header="0.3" footer="0.3"/>

</xml_diff>